<commit_message>
RSA Exp. 9 - Modificatins 4
</commit_message>
<xml_diff>
--- a/RSA_2019_08/X9_Data/x9KLDivs_simpleRSA_indOpt_all.xlsx
+++ b/RSA_2019_08/X9_Data/x9KLDivs_simpleRSA_indOpt_all.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="x9KLDivs_simpleRSA_indOpt_itera" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Iterative</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>min</t>
+  </si>
+  <si>
+    <t>NonIterative</t>
+  </si>
+  <si>
+    <t>IterParams</t>
+  </si>
+  <si>
+    <t>NonIterParams</t>
   </si>
 </sst>
 </file>
@@ -913,7 +922,7 @@
   <dimension ref="A1:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,6 +946,9 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
@@ -949,6 +961,9 @@
       <c r="K1" t="s">
         <v>12</v>
       </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
       <c r="M1" t="s">
         <v>6</v>
       </c>
@@ -960,6 +975,9 @@
       </c>
       <c r="P1" t="s">
         <v>9</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
       </c>
       <c r="R1" t="s">
         <v>13</v>
@@ -6440,7 +6458,7 @@
         <f>SUM(C2:C96)</f>
         <v>558.69335388268576</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="4">
         <f t="shared" ref="D100:U100" si="2">SUM(D2:D96)</f>
         <v>311.68378800808944</v>
       </c>
@@ -6448,7 +6466,7 @@
         <f t="shared" si="2"/>
         <v>105602.07683967038</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100" s="4">
         <f t="shared" si="2"/>
         <v>237.89047957572026</v>
       </c>
@@ -6456,7 +6474,7 @@
         <f t="shared" si="2"/>
         <v>558.69335388268576</v>
       </c>
-      <c r="I100" s="3">
+      <c r="I100" s="4">
         <f t="shared" si="2"/>
         <v>356.84690919179059</v>
       </c>
@@ -6464,7 +6482,7 @@
         <f t="shared" si="2"/>
         <v>94826.503358293092</v>
       </c>
-      <c r="K100" s="3">
+      <c r="K100" s="4">
         <f t="shared" si="2"/>
         <v>264.44960455884296</v>
       </c>

</xml_diff>

<commit_message>
Final (?) additions to CogSCi2020 RSA paper --- nearly good to go :-)
</commit_message>
<xml_diff>
--- a/RSA_2019_08/X9_Data/x9KLDivs_simpleRSA_indOpt_all.xlsx
+++ b/RSA_2019_08/X9_Data/x9KLDivs_simpleRSA_indOpt_all.xlsx
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A96" sqref="A2:U96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>